<commit_message>
AVL update from 3.35 to 3.37
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300_AVL/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/CS300_AVL/WEIGHTS/Weights.xlsx
@@ -115,37 +115,37 @@
     <t>WEIGHT ESTIMATION METHODS COMPARISON</t>
   </si>
   <si>
+    <t>ROSKAM</t>
+  </si>
+  <si>
+    <t>NICOLAI_1984</t>
+  </si>
+  <si>
+    <t>RAYMER</t>
+  </si>
+  <si>
+    <t>SADRAEY</t>
+  </si>
+  <si>
+    <t>JENKINSON</t>
+  </si>
+  <si>
+    <t>KROO</t>
+  </si>
+  <si>
     <t>TORENBEEK_1976</t>
   </si>
   <si>
     <t>TORENBEEK_2013</t>
   </si>
   <si>
-    <t>KROO</t>
-  </si>
-  <si>
-    <t>NICOLAI_1984</t>
-  </si>
-  <si>
-    <t>ROSKAM</t>
-  </si>
-  <si>
-    <t>SADRAEY</t>
-  </si>
-  <si>
-    <t>RAYMER</t>
-  </si>
-  <si>
-    <t>JENKINSON</t>
-  </si>
-  <si>
     <t>TORENBEEK_1982</t>
   </si>
   <si>
+    <t>NICOLAI_2013</t>
+  </si>
+  <si>
     <t>HOWE</t>
-  </si>
-  <si>
-    <t>NICOLAI_2013</t>
   </si>
   <si>
     <t>Total Reference Mass</t>
@@ -611,10 +611,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>10802.0</v>
+        <v>14190.0</v>
       </c>
       <c r="D8" t="n">
-        <v>71.78406059311477</v>
+        <v>125.66337898688195</v>
       </c>
     </row>
     <row r="9">
@@ -625,10 +625,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>7891.0</v>
+        <v>10196.0</v>
       </c>
       <c r="D9" t="n">
-        <v>25.49046677839925</v>
+        <v>62.14685075054604</v>
       </c>
     </row>
     <row r="10">
@@ -639,10 +639,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>7092.0</v>
+        <v>6416.0</v>
       </c>
       <c r="D10" t="n">
-        <v>12.783980533824291</v>
+        <v>2.0335616335330875</v>
       </c>
     </row>
     <row r="11">
@@ -653,10 +653,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>10196.0</v>
+        <v>6396.0</v>
       </c>
       <c r="D11" t="n">
-        <v>62.14685075054604</v>
+        <v>1.7155019027552412</v>
       </c>
     </row>
     <row r="12">
@@ -667,10 +667,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>14190.0</v>
+        <v>21031.0</v>
       </c>
       <c r="D12" t="n">
-        <v>125.66337898688195</v>
+        <v>234.45570989944426</v>
       </c>
     </row>
     <row r="13">
@@ -681,10 +681,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>6396.0</v>
+        <v>7092.0</v>
       </c>
       <c r="D13" t="n">
-        <v>1.7155019027552412</v>
+        <v>12.783980533824291</v>
       </c>
     </row>
     <row r="14">
@@ -695,10 +695,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>6416.0</v>
+        <v>10802.0</v>
       </c>
       <c r="D14" t="n">
-        <v>2.0335616335330875</v>
+        <v>71.78406059311477</v>
       </c>
     </row>
     <row r="15">
@@ -709,10 +709,10 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>21031.0</v>
+        <v>7891.0</v>
       </c>
       <c r="D15" t="n">
-        <v>234.45570989944426</v>
+        <v>25.49046677839925</v>
       </c>
     </row>
   </sheetData>
@@ -805,21 +805,21 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>6082.0</v>
+        <v>8327.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-8.752864028732963</v>
+        <v>24.928461235241798</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -847,16 +847,16 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>8327.0</v>
+        <v>6082.0</v>
       </c>
       <c r="D11" t="n">
-        <v>24.928461235241798</v>
+        <v>-8.752864028732963</v>
       </c>
     </row>
   </sheetData>
@@ -955,10 +955,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>1415.0</v>
+        <v>394.0</v>
       </c>
       <c r="D8" t="n">
-        <v>95.67587784810976</v>
+        <v>-45.51498524936025</v>
       </c>
     </row>
     <row r="9">
@@ -969,10 +969,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>52.0</v>
+        <v>1523.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-92.8090843476313</v>
+        <v>110.61085651072167</v>
       </c>
     </row>
     <row r="10">
@@ -983,52 +983,52 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>737.0</v>
+        <v>502.0</v>
       </c>
       <c r="D10" t="n">
-        <v>1.9174006883794317</v>
+        <v>-30.58000658674834</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>394.0</v>
+        <v>1040.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-45.51498524936025</v>
+        <v>43.81831304737396</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>1523.0</v>
+        <v>1415.0</v>
       </c>
       <c r="D12" t="n">
-        <v>110.61085651072167</v>
+        <v>95.67587784810976</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>1040.0</v>
+        <v>700.0</v>
       </c>
       <c r="D13" t="n">
-        <v>43.81831304737396</v>
+        <v>-3.199212371959834</v>
       </c>
     </row>
     <row r="14">
@@ -1039,24 +1039,24 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>502.0</v>
+        <v>52.0</v>
       </c>
       <c r="D14" t="n">
-        <v>-30.58000658674834</v>
+        <v>-92.8090843476313</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>700.0</v>
+        <v>737.0</v>
       </c>
       <c r="D15" t="n">
-        <v>-3.199212371959834</v>
+        <v>1.9174006883794317</v>
       </c>
     </row>
   </sheetData>
@@ -1149,72 +1149,72 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>1145.0</v>
+        <v>1523.0</v>
       </c>
       <c r="D8" t="n">
-        <v>58.338431191579986</v>
+        <v>110.61085651072167</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>124.0</v>
+        <v>179.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-82.85243190589003</v>
+        <v>-75.24665573511544</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>485.0</v>
+        <v>749.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-32.93088285771503</v>
+        <v>3.5768427620029772</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>1523.0</v>
+        <v>1145.0</v>
       </c>
       <c r="D11" t="n">
-        <v>110.61085651072167</v>
+        <v>58.338431191579986</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>749.0</v>
+        <v>502.0</v>
       </c>
       <c r="D12" t="n">
-        <v>3.5768427620029772</v>
+        <v>-30.58000658674834</v>
       </c>
     </row>
     <row r="13">
@@ -1225,24 +1225,24 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>179.0</v>
+        <v>124.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-75.24665573511544</v>
+        <v>-82.85243190589003</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>502.0</v>
+        <v>485.0</v>
       </c>
       <c r="D14" t="n">
-        <v>-30.58000658674834</v>
+        <v>-32.93088285771503</v>
       </c>
     </row>
   </sheetData>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -1591,44 +1591,44 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>2954.0</v>
+        <v>3265.0</v>
       </c>
       <c r="D11" t="n">
-        <v>13.19860779732021</v>
+        <v>25.116267589116617</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>3458.0</v>
+        <v>2954.0</v>
       </c>
       <c r="D12" t="n">
-        <v>32.51211434093882</v>
+        <v>13.19860779732021</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>3265.0</v>
+        <v>3458.0</v>
       </c>
       <c r="D13" t="n">
-        <v>25.116267589116617</v>
+        <v>32.51211434093882</v>
       </c>
     </row>
     <row r="14">
@@ -1663,44 +1663,44 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>2954.0</v>
+        <v>3265.0</v>
       </c>
       <c r="D18" t="n">
-        <v>13.19860779732021</v>
+        <v>25.116267589116617</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>3458.0</v>
+        <v>2954.0</v>
       </c>
       <c r="D19" t="n">
-        <v>32.51211434093882</v>
+        <v>13.19860779732021</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>3265.0</v>
+        <v>3458.0</v>
       </c>
       <c r="D20" t="n">
-        <v>25.116267589116617</v>
+        <v>32.51211434093882</v>
       </c>
     </row>
     <row r="21">
@@ -1814,7 +1814,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>

</xml_diff>